<commit_message>
Handle mid-quarter storage changes
</commit_message>
<xml_diff>
--- a/tests/resources/mock_storage_update_form.xlsx
+++ b/tests/resources/mock_storage_update_form.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bbanana@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBBB</t>
   </si>
 </sst>
 </file>
@@ -192,15 +204,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="21.57"/>
   </cols>
@@ -260,9 +272,36 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>44180.7005092593</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="ddurian@example.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="bbanana@example.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Fix column name discrepancy
</commit_message>
<xml_diff>
--- a/tests/resources/mock_storage_update_form.xlsx
+++ b/tests/resources/mock_storage_update_form.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Do you need separate access groups for specific projects?  If yes, please list the project names.</t>
   </si>
   <si>
-    <t xml:space="preserve">By clicking yes below, you agree with these general terms.</t>
+    <t xml:space="preserve">By clicking yes below, you agree with these general terms. </t>
   </si>
   <si>
     <t xml:space="preserve">Optional: Please feel free to leave any feedback.</t>
@@ -230,10 +230,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="21.57"/>
   </cols>

</xml_diff>

<commit_message>
Fix tests for new storage policy
Also, there was a typo in the user update form.
</commit_message>
<xml_diff>
--- a/tests/resources/mock_storage_update_form.xlsx
+++ b/tests/resources/mock_storage_update_form.xlsx
@@ -230,10 +230,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="21.57"/>
   </cols>
@@ -298,7 +298,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
-        <v>44180.7005092593</v>
+        <v>44150.7005092593</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>16</v>
@@ -370,8 +370,8 @@
     <hyperlink ref="B5" r:id="rId4" display="jjackfruit@example.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Use new storage update text
</commit_message>
<xml_diff>
--- a/tests/resources/mock_storage_update_form.xlsx
+++ b/tests/resources/mock_storage_update_form.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Last name</t>
   </si>
   <si>
-    <t xml:space="preserve">Required storage needs (in TB)</t>
+    <t xml:space="preserve">Additional storage needs (in TB; to be added to existing storage)</t>
   </si>
   <si>
     <t xml:space="preserve">Speed code</t>
@@ -230,10 +230,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="21.57"/>
   </cols>

</xml_diff>

<commit_message>
Handle updated speed codes
</commit_message>
<xml_diff>
--- a/tests/resources/mock_storage_update_form.xlsx
+++ b/tests/resources/mock_storage_update_form.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Banana</t>
   </si>
   <si>
-    <t xml:space="preserve">BBBB</t>
+    <t xml:space="preserve">BBBC</t>
   </si>
   <si>
     <t xml:space="preserve">wwatermelon@example.com</t>
@@ -230,10 +230,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="21.57"/>
   </cols>

</xml_diff>